<commit_message>
end of first pass through analyses prior to SAF convention
</commit_message>
<xml_diff>
--- a/stats-residual basal area 2019 harvest x location.xlsx
+++ b/stats-residual basal area 2019 harvest x location.xlsx
@@ -67,7 +67,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -111,7 +111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:D16"/>
+  <dimension ref="B4:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F12" sqref="F12:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +410,7 @@
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -421,7 +421,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -432,7 +432,7 @@
         <v>34.761904761904802</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -443,7 +443,7 @@
         <v>23.75</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -454,7 +454,7 @@
         <v>38.529411764705898</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -465,7 +465,7 @@
         <v>30.588235294117599</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -475,8 +475,9 @@
       <c r="D9" s="2">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -486,8 +487,9 @@
       <c r="D10" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -498,7 +500,7 @@
         <v>18.275862068965498</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -508,8 +510,11 @@
       <c r="D12" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F12" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -519,8 +524,11 @@
       <c r="D13" s="2">
         <v>1.5384615384615401</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F13" s="2">
+        <v>1.5384615384615401</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -530,8 +538,11 @@
       <c r="D14" s="2">
         <v>39.285714285714299</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F14" s="2">
+        <v>18.275862068965498</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -542,7 +553,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>11</v>
       </c>

</xml_diff>